<commit_message>
Egy formra rendezve, beolvasáskor numeric típust értelmezi
</commit_message>
<xml_diff>
--- a/MyDataGrid/tabella_2.xlsx
+++ b/MyDataGrid/tabella_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gmiskola-my.sharepoint.com/personal/kovacszsolt100_gmiskola_hu/Documents/Programozás/DotNetBackend2/MyDataGrid/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2EACA719-664B-41EC-B340-ECB6FEF2C0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{2EACA719-664B-41EC-B340-ECB6FEF2C0D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{456E46DF-33A4-4641-B4CD-507804C6B172}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{74C724F2-1C39-4FB1-9D3C-7742ADBC4DAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{74C724F2-1C39-4FB1-9D3C-7742ADBC4DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Bács-Kiskun" sheetId="1" r:id="rId1"/>
@@ -305,27 +305,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -335,6 +322,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -353,6 +343,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -670,526 +672,524 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304E3272-341E-45DF-9C1B-654A4CD281AD}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="4"/>
-    <col min="2" max="2" width="20.21875" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="4"/>
+    <col min="2" max="2" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>14</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>9</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>3</v>
       </c>
-      <c r="F2" s="5">
-        <v>2</v>
-      </c>
-      <c r="G2" s="5">
+      <c r="F2" s="4">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
         <v>36</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>11</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>25</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="6">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="13.8" customHeight="1">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4">
         <v>14</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>4</v>
       </c>
-      <c r="F3" s="5">
-        <v>2</v>
-      </c>
-      <c r="G3" s="5">
+      <c r="F3" s="4">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4">
         <v>21</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="4">
         <v>9</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="4">
         <v>12</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="6">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>14</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>7</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>3</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>4</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>28</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H4" s="4">
         <v>18</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="4">
         <v>10</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>14</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>7</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>3</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>4</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>24</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H5" s="4">
         <v>22</v>
       </c>
-      <c r="I5" s="5">
-        <v>2</v>
-      </c>
-      <c r="J5" s="7">
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="6">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>14</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>6</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>4</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>4</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>21</v>
       </c>
-      <c r="H6" s="5">
+      <c r="H6" s="4">
         <v>23</v>
       </c>
-      <c r="I6" s="5">
+      <c r="I6" s="4">
         <v>-2</v>
       </c>
-      <c r="J6" s="7">
+      <c r="J6" s="6">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>14</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>6</v>
       </c>
-      <c r="E7" s="5">
-        <v>2</v>
-      </c>
-      <c r="F7" s="5">
+      <c r="E7" s="4">
+        <v>2</v>
+      </c>
+      <c r="F7" s="4">
         <v>6</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G7" s="4">
         <v>27</v>
       </c>
-      <c r="H7" s="5">
+      <c r="H7" s="4">
         <v>20</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I7" s="4">
         <v>7</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>14</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>6</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>1</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>7</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="4">
         <v>23</v>
       </c>
-      <c r="H8" s="5">
+      <c r="H8" s="4">
         <v>29</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="4">
         <v>-6</v>
       </c>
-      <c r="J8" s="7">
+      <c r="J8" s="6">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>14</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>3</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>6</v>
       </c>
-      <c r="G9" s="5">
+      <c r="G9" s="4">
         <v>36</v>
       </c>
-      <c r="H9" s="5">
+      <c r="H9" s="4">
         <v>29</v>
       </c>
-      <c r="I9" s="5">
+      <c r="I9" s="4">
         <v>7</v>
       </c>
-      <c r="J9" s="7">
+      <c r="J9" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>13</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>5</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>3</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>5</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <v>18</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H10" s="4">
         <v>18</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I10" s="4">
         <v>0</v>
       </c>
-      <c r="J10" s="7">
+      <c r="J10" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>12</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>5</v>
       </c>
-      <c r="E11" s="5">
-        <v>2</v>
-      </c>
-      <c r="F11" s="5">
+      <c r="E11" s="4">
+        <v>2</v>
+      </c>
+      <c r="F11" s="4">
         <v>5</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>38</v>
       </c>
-      <c r="H11" s="5">
+      <c r="H11" s="4">
         <v>25</v>
       </c>
-      <c r="I11" s="5">
+      <c r="I11" s="4">
         <v>13</v>
       </c>
-      <c r="J11" s="7">
+      <c r="J11" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>13</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>5</v>
       </c>
-      <c r="E12" s="5">
-        <v>2</v>
-      </c>
-      <c r="F12" s="5">
+      <c r="E12" s="4">
+        <v>2</v>
+      </c>
+      <c r="F12" s="4">
         <v>6</v>
       </c>
-      <c r="G12" s="5">
-        <v>16</v>
-      </c>
-      <c r="H12" s="5">
+      <c r="G12" s="4">
+        <v>16</v>
+      </c>
+      <c r="H12" s="4">
         <v>19</v>
       </c>
-      <c r="I12" s="5">
+      <c r="I12" s="4">
         <v>-3</v>
       </c>
-      <c r="J12" s="7">
+      <c r="J12" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="5">
+      <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>14</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>5</v>
       </c>
-      <c r="E13" s="5">
-        <v>2</v>
-      </c>
-      <c r="F13" s="5">
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4">
         <v>7</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>18</v>
       </c>
-      <c r="H13" s="5">
+      <c r="H13" s="4">
         <v>29</v>
       </c>
-      <c r="I13" s="5">
+      <c r="I13" s="4">
         <v>-11</v>
       </c>
-      <c r="J13" s="7">
+      <c r="J13" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>14</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>4</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>5</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>5</v>
       </c>
-      <c r="G14" s="5">
-        <v>16</v>
-      </c>
-      <c r="H14" s="5">
-        <v>16</v>
-      </c>
-      <c r="I14" s="5">
+      <c r="G14" s="4">
+        <v>16</v>
+      </c>
+      <c r="H14" s="4">
+        <v>16</v>
+      </c>
+      <c r="I14" s="4">
         <v>0</v>
       </c>
-      <c r="J14" s="7">
+      <c r="J14" s="6">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="5">
+      <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>14</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>4</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>1</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>9</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <v>22</v>
       </c>
-      <c r="H15" s="5">
+      <c r="H15" s="4">
         <v>48</v>
       </c>
-      <c r="I15" s="5">
+      <c r="I15" s="4">
         <v>-26</v>
       </c>
-      <c r="J15" s="7">
+      <c r="J15" s="6">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>15</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>14</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="7">
         <v>1</v>
       </c>
-      <c r="E16" s="8">
-        <v>2</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="E16" s="7">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7">
         <v>11</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="7">
         <v>18</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>46</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="7">
         <v>-28</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="9">
         <v>5</v>
       </c>
     </row>
@@ -1212,354 +1212,354 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1">
-      <c r="A2" s="12">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="7">
         <v>11</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="7">
         <v>10</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="7">
         <v>42</v>
       </c>
-      <c r="H2" s="12">
-        <v>2</v>
-      </c>
-      <c r="I2" s="12">
+      <c r="H2" s="7">
+        <v>2</v>
+      </c>
+      <c r="I2" s="7">
         <v>40</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="9">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1">
-      <c r="A3" s="18">
-        <v>2</v>
-      </c>
-      <c r="B3" s="19" t="s">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="14">
         <v>11</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="14">
         <v>8</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="14">
         <v>1</v>
       </c>
-      <c r="F3" s="18">
-        <v>2</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="F3" s="14">
+        <v>2</v>
+      </c>
+      <c r="G3" s="14">
         <v>31</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="14">
         <v>17</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="14">
         <v>14</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="16">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15" thickBot="1">
-      <c r="A4" s="18">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="14">
         <v>11</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="14">
         <v>7</v>
       </c>
-      <c r="E4" s="18">
-        <v>2</v>
-      </c>
-      <c r="F4" s="18">
-        <v>2</v>
-      </c>
-      <c r="G4" s="18">
+      <c r="E4" s="14">
+        <v>2</v>
+      </c>
+      <c r="F4" s="14">
+        <v>2</v>
+      </c>
+      <c r="G4" s="14">
         <v>30</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>9</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
         <v>21</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="16">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" thickBot="1">
-      <c r="A5" s="18">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="14">
         <v>11</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="14">
         <v>7</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="14">
         <v>0</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="14">
         <v>4</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="14">
         <v>26</v>
       </c>
-      <c r="H5" s="18">
-        <v>16</v>
-      </c>
-      <c r="I5" s="18">
+      <c r="H5" s="14">
+        <v>16</v>
+      </c>
+      <c r="I5" s="14">
         <v>10</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="16">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1">
-      <c r="A6" s="18">
+      <c r="A6" s="14">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="14">
         <v>11</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="14">
         <v>6</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="14">
         <v>3</v>
       </c>
-      <c r="F6" s="18">
-        <v>2</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="F6" s="14">
+        <v>2</v>
+      </c>
+      <c r="G6" s="14">
         <v>30</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="14">
         <v>17</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="14">
         <v>13</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="16">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" thickBot="1">
-      <c r="A7" s="18">
+      <c r="A7" s="14">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="14">
         <v>11</v>
       </c>
-      <c r="D7" s="18">
-        <v>2</v>
-      </c>
-      <c r="E7" s="18">
+      <c r="D7" s="14">
+        <v>2</v>
+      </c>
+      <c r="E7" s="14">
         <v>4</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="14">
         <v>5</v>
       </c>
-      <c r="G7" s="18">
-        <v>16</v>
-      </c>
-      <c r="H7" s="18">
+      <c r="G7" s="14">
+        <v>16</v>
+      </c>
+      <c r="H7" s="14">
         <v>27</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>-11</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="16">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1">
-      <c r="A8" s="18">
+      <c r="A8" s="14">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <v>11</v>
       </c>
-      <c r="D8" s="18">
-        <v>2</v>
-      </c>
-      <c r="E8" s="18">
-        <v>2</v>
-      </c>
-      <c r="F8" s="18">
+      <c r="D8" s="14">
+        <v>2</v>
+      </c>
+      <c r="E8" s="14">
+        <v>2</v>
+      </c>
+      <c r="F8" s="14">
         <v>7</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <v>19</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="14">
         <v>31</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="14">
         <v>-12</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1">
-      <c r="A9" s="18">
+      <c r="A9" s="14">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="14">
         <v>11</v>
       </c>
-      <c r="D9" s="18">
-        <v>2</v>
-      </c>
-      <c r="E9" s="18">
+      <c r="D9" s="14">
+        <v>2</v>
+      </c>
+      <c r="E9" s="14">
         <v>0</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="14">
         <v>9</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="14">
         <v>9</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="14">
         <v>31</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="14">
         <v>-22</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="16">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="18">
+      <c r="A10" s="14">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="14">
         <v>11</v>
       </c>
-      <c r="D10" s="18">
-        <v>2</v>
-      </c>
-      <c r="E10" s="18">
+      <c r="D10" s="14">
+        <v>2</v>
+      </c>
+      <c r="E10" s="14">
         <v>0</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="14">
         <v>9</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <v>14</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <v>50</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="14">
         <v>-36</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="16">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1">
-      <c r="A11" s="15">
+      <c r="A11" s="11">
         <v>10</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="11">
         <v>11</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="11">
         <v>1</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="11">
         <v>3</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="11">
         <v>7</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="11">
         <v>15</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="11">
         <v>32</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="11">
         <v>-17</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="13">
         <v>6</v>
       </c>
     </row>
@@ -1572,9 +1572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F9AC39-4AB1-4D2D-9A9C-2338BD8A4B28}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -1582,66 +1580,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="I1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1">
-      <c r="A2" s="12">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="12">
-        <v>16</v>
-      </c>
-      <c r="D2" s="12">
+      <c r="C2" s="7">
+        <v>16</v>
+      </c>
+      <c r="D2" s="7">
         <v>15</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="7">
         <v>50</v>
       </c>
-      <c r="H2" s="12">
+      <c r="H2" s="7">
         <v>7</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="7">
         <v>43</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="9">
         <v>46</v>
       </c>
     </row>
@@ -1649,31 +1647,31 @@
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="18">
-        <v>16</v>
-      </c>
-      <c r="D3" s="18">
+      <c r="C3" s="14">
+        <v>16</v>
+      </c>
+      <c r="D3" s="14">
         <v>10</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="14">
         <v>4</v>
       </c>
-      <c r="F3" s="18">
-        <v>2</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="F3" s="14">
+        <v>2</v>
+      </c>
+      <c r="G3" s="14">
         <v>33</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="14">
         <v>13</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="14">
         <v>20</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="16">
         <v>34</v>
       </c>
     </row>
@@ -1681,31 +1679,31 @@
       <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="18">
-        <v>16</v>
-      </c>
-      <c r="D4" s="18">
+      <c r="C4" s="14">
+        <v>16</v>
+      </c>
+      <c r="D4" s="14">
         <v>10</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="14">
         <v>3</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="14">
         <v>3</v>
       </c>
-      <c r="G4" s="18">
+      <c r="G4" s="14">
         <v>40</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="14">
         <v>20</v>
       </c>
-      <c r="I4" s="18">
+      <c r="I4" s="14">
         <v>20</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="16">
         <v>33</v>
       </c>
     </row>
@@ -1713,31 +1711,31 @@
       <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="18">
-        <v>16</v>
-      </c>
-      <c r="D5" s="18">
+      <c r="C5" s="14">
+        <v>16</v>
+      </c>
+      <c r="D5" s="14">
         <v>9</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="14">
         <v>3</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="14">
         <v>4</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="14">
         <v>34</v>
       </c>
-      <c r="H5" s="18">
+      <c r="H5" s="14">
         <v>22</v>
       </c>
-      <c r="I5" s="18">
+      <c r="I5" s="14">
         <v>12</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="16">
         <v>30</v>
       </c>
     </row>
@@ -1745,31 +1743,31 @@
       <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="18">
-        <v>16</v>
-      </c>
-      <c r="D6" s="18">
+      <c r="C6" s="14">
+        <v>16</v>
+      </c>
+      <c r="D6" s="14">
         <v>8</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="14">
         <v>0</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="14">
         <v>8</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="14">
         <v>24</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="14">
         <v>23</v>
       </c>
-      <c r="I6" s="18">
+      <c r="I6" s="14">
         <v>1</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="16">
         <v>24</v>
       </c>
     </row>
@@ -1777,31 +1775,31 @@
       <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="18">
-        <v>16</v>
-      </c>
-      <c r="D7" s="18">
+      <c r="C7" s="14">
+        <v>16</v>
+      </c>
+      <c r="D7" s="14">
         <v>6</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="14">
         <v>4</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="14">
         <v>6</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="14">
         <v>27</v>
       </c>
-      <c r="H7" s="18">
+      <c r="H7" s="14">
         <v>36</v>
       </c>
-      <c r="I7" s="18">
+      <c r="I7" s="14">
         <v>-9</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="16">
         <v>22</v>
       </c>
     </row>
@@ -1809,31 +1807,31 @@
       <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <v>15</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <v>6</v>
       </c>
-      <c r="E8" s="18">
-        <v>2</v>
-      </c>
-      <c r="F8" s="18">
+      <c r="E8" s="14">
+        <v>2</v>
+      </c>
+      <c r="F8" s="14">
         <v>7</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G8" s="14">
         <v>25</v>
       </c>
-      <c r="H8" s="18">
+      <c r="H8" s="14">
         <v>23</v>
       </c>
-      <c r="I8" s="18">
-        <v>2</v>
-      </c>
-      <c r="J8" s="20">
+      <c r="I8" s="14">
+        <v>2</v>
+      </c>
+      <c r="J8" s="16">
         <v>20</v>
       </c>
     </row>
@@ -1841,31 +1839,31 @@
       <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="18">
-        <v>16</v>
-      </c>
-      <c r="D9" s="18">
+      <c r="C9" s="14">
+        <v>16</v>
+      </c>
+      <c r="D9" s="14">
         <v>6</v>
       </c>
-      <c r="E9" s="18">
-        <v>2</v>
-      </c>
-      <c r="F9" s="18">
+      <c r="E9" s="14">
+        <v>2</v>
+      </c>
+      <c r="F9" s="14">
         <v>8</v>
       </c>
-      <c r="G9" s="18">
+      <c r="G9" s="14">
         <v>28</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="14">
         <v>35</v>
       </c>
-      <c r="I9" s="18">
+      <c r="I9" s="14">
         <v>-7</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="16">
         <v>20</v>
       </c>
     </row>
@@ -1873,31 +1871,31 @@
       <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="18">
-        <v>16</v>
-      </c>
-      <c r="D10" s="18">
+      <c r="C10" s="14">
+        <v>16</v>
+      </c>
+      <c r="D10" s="14">
         <v>6</v>
       </c>
-      <c r="E10" s="18">
-        <v>2</v>
-      </c>
-      <c r="F10" s="18">
+      <c r="E10" s="14">
+        <v>2</v>
+      </c>
+      <c r="F10" s="14">
         <v>8</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="14">
         <v>24</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="14">
         <v>35</v>
       </c>
-      <c r="I10" s="18">
+      <c r="I10" s="14">
         <v>-11</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="16">
         <v>20</v>
       </c>
     </row>
@@ -1905,31 +1903,31 @@
       <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="18">
-        <v>16</v>
-      </c>
-      <c r="D11" s="18">
+      <c r="C11" s="14">
+        <v>16</v>
+      </c>
+      <c r="D11" s="14">
         <v>6</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="14">
         <v>1</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="14">
         <v>9</v>
       </c>
-      <c r="G11" s="18">
+      <c r="G11" s="14">
         <v>23</v>
       </c>
-      <c r="H11" s="18">
+      <c r="H11" s="14">
         <v>36</v>
       </c>
-      <c r="I11" s="18">
+      <c r="I11" s="14">
         <v>-13</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="16">
         <v>19</v>
       </c>
     </row>
@@ -1937,31 +1935,31 @@
       <c r="A12" s="18">
         <v>11</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="18">
-        <v>16</v>
-      </c>
-      <c r="D12" s="18">
+      <c r="C12" s="14">
+        <v>16</v>
+      </c>
+      <c r="D12" s="14">
         <v>5</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="14">
         <v>4</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="14">
         <v>7</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="14">
         <v>29</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="14">
         <v>28</v>
       </c>
-      <c r="I12" s="18">
+      <c r="I12" s="14">
         <v>1</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="16">
         <v>19</v>
       </c>
     </row>
@@ -1969,31 +1967,31 @@
       <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="14">
         <v>15</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="14">
         <v>5</v>
       </c>
-      <c r="E13" s="18">
-        <v>2</v>
-      </c>
-      <c r="F13" s="18">
+      <c r="E13" s="14">
+        <v>2</v>
+      </c>
+      <c r="F13" s="14">
         <v>8</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="14">
         <v>24</v>
       </c>
-      <c r="H13" s="18">
+      <c r="H13" s="14">
         <v>26</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="14">
         <v>-2</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="16">
         <v>17</v>
       </c>
     </row>
@@ -2001,31 +1999,31 @@
       <c r="A14" s="18">
         <v>13</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="18">
-        <v>16</v>
-      </c>
-      <c r="D14" s="18">
+      <c r="C14" s="14">
+        <v>16</v>
+      </c>
+      <c r="D14" s="14">
         <v>5</v>
       </c>
-      <c r="E14" s="18">
-        <v>2</v>
-      </c>
-      <c r="F14" s="18">
+      <c r="E14" s="14">
+        <v>2</v>
+      </c>
+      <c r="F14" s="14">
         <v>9</v>
       </c>
-      <c r="G14" s="18">
+      <c r="G14" s="14">
         <v>19</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="14">
         <v>29</v>
       </c>
-      <c r="I14" s="18">
+      <c r="I14" s="14">
         <v>-10</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="16">
         <v>17</v>
       </c>
     </row>
@@ -2033,31 +2031,31 @@
       <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="18">
-        <v>16</v>
-      </c>
-      <c r="D15" s="18">
+      <c r="C15" s="14">
+        <v>16</v>
+      </c>
+      <c r="D15" s="14">
         <v>5</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="14">
         <v>0</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="14">
         <v>11</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="14">
         <v>36</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="14">
         <v>46</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="14">
         <v>-10</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="16">
         <v>15</v>
       </c>
     </row>
@@ -2065,36 +2063,36 @@
       <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="18">
-        <v>16</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="C16" s="14">
+        <v>16</v>
+      </c>
+      <c r="D16" s="14">
         <v>4</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="14">
         <v>3</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="14">
         <v>9</v>
       </c>
-      <c r="G16" s="18">
+      <c r="G16" s="14">
         <v>25</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="14">
         <v>36</v>
       </c>
-      <c r="I16" s="18">
+      <c r="I16" s="14">
         <v>-11</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="16">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" thickBot="1">
-      <c r="A17" s="1">
+      <c r="A17" s="19">
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">

</xml_diff>